<commit_message>
Entrega Ejemplo – laboratorio 4
</commit_message>
<xml_diff>
--- a/Docs/Tablas Lab 4 Maquina 1.xlsx
+++ b/Docs/Tablas Lab 4 Maquina 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes.sharepoint.com/sites/ISIS1225/Documentos compartidos/General/202110/Laboratorios/Lab 04 - Ordenamientos Iterativos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole/Desktop/ESTRUCTURA DE DATOS/LABORATORIOS/LabSorts-S04-G07/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="8_{A25BB2A9-7879-4ABF-A93E-5BD797619927}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3E197636-5D23-49AC-AB0F-C814FF421F77}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DDAF3D-691F-BB46-9729-B69CCE6D4599}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15586" activeTab="5" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25780" windowHeight="15580" activeTab="1" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab4" sheetId="1" r:id="rId1"/>
@@ -24,15 +24,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -84,7 +75,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -526,7 +517,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -613,7 +604,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -664,34 +655,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>563.12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>2293.0100000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>9248.66</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>38467.51</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>164240.64000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>688699.79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -781,7 +760,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -832,34 +811,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>645.57000000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2593.0700000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>10749.37</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>45474.61</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>190602.47</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>89</c:v>
+                  <c:v>749434.38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -948,7 +915,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -999,34 +966,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>36.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>77.56</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>171.08</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>417.92</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>913.15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59</c:v>
+                  <c:v>2158.0700000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69</c:v>
+                  <c:v>5339.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79</c:v>
+                  <c:v>12081.23</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>99</c:v>
+                  <c:v>31470.36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1126,7 +1090,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1164,7 +1128,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -1248,7 +1212,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1286,7 +1250,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -1328,7 +1292,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1365,7 +1329,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1441,7 +1405,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1528,7 +1492,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1579,34 +1543,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>44019.46</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>362439.99</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>140</c:v>
+                  <c:v>2996884.79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1696,7 +1639,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1708,34 +1651,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>39137.78</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>321500.03999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>178</c:v>
+                  <c:v>2615806.89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1747,34 +1669,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>39137.78</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>321500.03999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>178</c:v>
+                  <c:v>2615806.89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1863,7 +1764,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1914,34 +1815,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>2196.17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>10308.120000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88</c:v>
+                  <c:v>48337.59</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
+                  <c:v>241678.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>118</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>158</c:v>
+                  <c:v>1075527.6100000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2041,7 +1927,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2079,7 +1965,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -2163,7 +2049,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2201,7 +2087,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -2243,7 +2129,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2280,7 +2166,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -2356,7 +2242,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2444,7 +2330,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2495,34 +2381,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>563.12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>2293.0100000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>9248.66</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>38467.51</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>164240.64000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>688699.79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2612,7 +2486,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2663,34 +2537,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>44019.46</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>362439.99</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>140</c:v>
+                  <c:v>2996884.79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2790,7 +2643,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2828,7 +2681,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -2907,7 +2760,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2945,7 +2798,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -2987,7 +2840,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3024,7 +2877,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -3095,7 +2948,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3183,7 +3036,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3234,34 +3087,22 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>645.57000000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2593.0700000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>10749.37</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>45474.61</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>190602.47</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>89</c:v>
+                  <c:v>749434.38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3351,7 +3192,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3402,34 +3243,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>39137.78</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>321500.03999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>178</c:v>
+                  <c:v>2615806.89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3529,7 +3349,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3567,7 +3387,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -3646,7 +3466,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3684,7 +3504,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -3726,7 +3546,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3763,7 +3583,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -3834,7 +3654,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3922,7 +3742,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3973,34 +3793,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>36.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>77.56</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>171.08</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>417.92</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>913.15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59</c:v>
+                  <c:v>2158.0700000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69</c:v>
+                  <c:v>5339.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79</c:v>
+                  <c:v>12081.23</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>99</c:v>
+                  <c:v>31470.36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4090,7 +3907,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4141,34 +3958,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>2196.17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>10308.120000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88</c:v>
+                  <c:v>48337.59</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
+                  <c:v>241678.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>118</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>158</c:v>
+                  <c:v>1075527.6100000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4268,7 +4070,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4306,7 +4108,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -4385,7 +4187,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4423,7 +4225,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -4465,7 +4267,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4502,7 +4304,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -7286,7 +7088,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{BF2A59F4-6CD8-490D-818C-7B3BB3F2B140}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7297,7 +7099,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{0D09CF8B-80E2-4734-A9D4-9F6060F1BA3D}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7308,7 +7110,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3D4D373F-B89D-476A-916E-D6B8B50B0AC1}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7319,7 +7121,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{662C0436-FCD4-45AD-AA7D-093158D92847}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7330,7 +7132,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{39C68510-AE01-4761-A7FB-5F1B76E923F7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7341,7 +7143,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="8669130" cy="6272696"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7374,7 +7176,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="8669130" cy="6272696"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7407,7 +7209,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="8669130" cy="6272696"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7440,7 +7242,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="8669130" cy="6272696"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7473,7 +7275,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="8669130" cy="6272696"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7828,18 +7630,18 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.1171875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.52734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.76171875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="16">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -7853,164 +7655,129 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
       <c r="B2" s="4">
-        <v>10</v>
+        <v>563.12</v>
       </c>
       <c r="C2" s="4">
-        <v>1</v>
+        <v>645.57000000000005</v>
       </c>
       <c r="D2" s="4">
-        <v>4</v>
+        <v>36.700000000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>2000</v>
       </c>
       <c r="B3" s="4">
-        <v>20</v>
+        <v>2293.0100000000002</v>
       </c>
       <c r="C3" s="4">
-        <v>2</v>
+        <v>2593.0700000000002</v>
       </c>
       <c r="D3" s="4">
-        <f>D2+15</f>
-        <v>19</v>
+        <v>77.56</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>4000</v>
       </c>
       <c r="B4" s="4">
-        <v>30</v>
+        <v>9248.66</v>
       </c>
       <c r="C4" s="4">
-        <f>C3+C2</f>
-        <v>3</v>
+        <v>10749.37</v>
       </c>
       <c r="D4" s="4">
-        <f t="shared" ref="D4:D11" si="0">D3+10</f>
-        <v>29</v>
+        <v>171.08</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>8000</v>
       </c>
       <c r="B5" s="4">
-        <v>40</v>
+        <v>38467.51</v>
       </c>
       <c r="C5" s="4">
-        <f t="shared" ref="C5:C11" si="1">C4+C3</f>
-        <v>5</v>
+        <v>45474.61</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" si="0"/>
-        <v>39</v>
+        <v>417.92</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>16000</v>
       </c>
       <c r="B6" s="4">
-        <v>50</v>
+        <v>164240.64000000001</v>
       </c>
       <c r="C6" s="4">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <v>190602.47</v>
       </c>
       <c r="D6" s="4">
-        <f t="shared" si="0"/>
-        <v>49</v>
+        <v>913.15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>32000</v>
       </c>
       <c r="B7" s="4">
-        <v>60</v>
+        <v>688699.79</v>
       </c>
       <c r="C7" s="4">
-        <f t="shared" si="1"/>
-        <v>13</v>
+        <v>749434.38</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" si="0"/>
-        <v>59</v>
+        <v>2158.0700000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>64000</v>
       </c>
-      <c r="B8" s="4">
-        <v>70</v>
-      </c>
-      <c r="C8" s="4">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="4">
-        <f t="shared" si="0"/>
-        <v>69</v>
+        <v>5339.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>128000</v>
       </c>
-      <c r="B9" s="4">
-        <v>80</v>
-      </c>
-      <c r="C9" s="4">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
       <c r="D9" s="4">
-        <f t="shared" si="0"/>
-        <v>79</v>
+        <v>12081.23</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>256000</v>
       </c>
-      <c r="B10" s="4">
-        <v>90</v>
-      </c>
-      <c r="C10" s="4">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="4">
-        <f t="shared" si="0"/>
-        <v>89</v>
+        <v>31470.36</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>512000</v>
       </c>
-      <c r="B11" s="4">
-        <v>100</v>
-      </c>
-      <c r="C11" s="4">
-        <f t="shared" si="1"/>
-        <v>89</v>
-      </c>
-      <c r="D11" s="4">
-        <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:4" ht="16">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -8024,162 +7791,107 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>1000</v>
       </c>
       <c r="B15" s="4">
-        <v>50</v>
+        <v>44019.46</v>
       </c>
       <c r="C15" s="4">
-        <v>2</v>
+        <v>39137.78</v>
       </c>
       <c r="D15" s="4">
-        <v>35</v>
+        <v>2196.17</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:4">
       <c r="A16" s="1">
         <v>2000</v>
       </c>
       <c r="B16" s="4">
-        <v>60</v>
+        <v>362439.99</v>
       </c>
       <c r="C16" s="4">
-        <v>4</v>
+        <v>321500.03999999998</v>
       </c>
       <c r="D16" s="4">
-        <f>D15+43</f>
-        <v>78</v>
+        <v>10308.120000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>4000</v>
       </c>
       <c r="B17" s="4">
-        <v>70</v>
+        <v>2996884.79</v>
       </c>
       <c r="C17" s="4">
-        <f t="shared" ref="C17:C24" si="2">C16+C15</f>
-        <v>6</v>
+        <v>2615806.89</v>
       </c>
       <c r="D17" s="4">
-        <f t="shared" ref="D17:D24" si="3">D16+10</f>
-        <v>88</v>
+        <v>48337.59</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>8000</v>
       </c>
-      <c r="B18" s="4">
-        <v>80</v>
-      </c>
-      <c r="C18" s="4">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
       <c r="D18" s="4">
-        <f t="shared" si="3"/>
-        <v>98</v>
+        <v>241678.25</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>16000</v>
       </c>
-      <c r="B19" s="4">
-        <v>90</v>
-      </c>
-      <c r="C19" s="4">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
       <c r="D19" s="4">
-        <f t="shared" si="3"/>
-        <v>108</v>
+        <v>1075527.6100000001</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>32000</v>
       </c>
-      <c r="B20" s="4">
-        <v>100</v>
-      </c>
-      <c r="C20" s="4">
-        <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="D20" s="4">
-        <f t="shared" si="3"/>
-        <v>118</v>
-      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>64000</v>
       </c>
-      <c r="B21" s="4">
-        <v>110</v>
-      </c>
-      <c r="C21" s="4">
-        <f t="shared" si="2"/>
-        <v>42</v>
-      </c>
-      <c r="D21" s="4">
-        <f t="shared" si="3"/>
-        <v>128</v>
-      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>128000</v>
       </c>
-      <c r="B22" s="4">
-        <v>120</v>
-      </c>
-      <c r="C22" s="4">
-        <f t="shared" si="2"/>
-        <v>68</v>
-      </c>
-      <c r="D22" s="4">
-        <f t="shared" si="3"/>
-        <v>138</v>
-      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>256000</v>
       </c>
-      <c r="B23" s="4">
-        <v>130</v>
-      </c>
-      <c r="C23" s="4">
-        <f t="shared" si="2"/>
-        <v>110</v>
-      </c>
-      <c r="D23" s="4">
-        <f t="shared" si="3"/>
-        <v>148</v>
-      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>512000</v>
       </c>
-      <c r="B24" s="4">
-        <v>140</v>
-      </c>
-      <c r="C24" s="4">
-        <f t="shared" si="2"/>
-        <v>178</v>
-      </c>
-      <c r="D24" s="4">
-        <f t="shared" si="3"/>
-        <v>158</v>
-      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8191,12 +7903,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8411,15 +8120,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8444,10 +8157,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>